<commit_message>
Added python-twitter & modified allowed hosts
</commit_message>
<xml_diff>
--- a/doc/AllowedHosts.xlsx
+++ b/doc/AllowedHosts.xlsx
@@ -19,35 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
-  <si>
-    <t>107.19.180.14</t>
-  </si>
-  <si>
-    <t>108.35.130.213</t>
-  </si>
-  <si>
-    <t>108.88.37.242</t>
-  </si>
-  <si>
-    <t>142.255.66.%</t>
-  </si>
-  <si>
-    <t>142.255.72.1</t>
-  </si>
-  <si>
-    <t>142.255.89.169</t>
-  </si>
-  <si>
-    <t>142.255.92.%</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>155.246.138.82</t>
   </si>
   <si>
-    <t>155.246.5.%</t>
-  </si>
-  <si>
     <t>155.246.61.9</t>
   </si>
   <si>
@@ -57,54 +33,18 @@
     <t>156.56.90.114</t>
   </si>
   <si>
-    <t>184.152.69.62</t>
-  </si>
-  <si>
-    <t>208.125.28.94</t>
-  </si>
-  <si>
-    <t>24.193.82.205</t>
-  </si>
-  <si>
-    <t>24.22.177.253</t>
-  </si>
-  <si>
-    <t>68.161.244.32</t>
-  </si>
-  <si>
     <t>69.174.48.81</t>
   </si>
   <si>
-    <t>70.39.146.73</t>
-  </si>
-  <si>
-    <t>76.100.117.111</t>
-  </si>
-  <si>
     <t>98.233.61.21</t>
   </si>
   <si>
-    <t>99.25.74.167</t>
-  </si>
-  <si>
-    <t>cpe-24-193-82-187.nyc.res.rr.com</t>
-  </si>
-  <si>
-    <t>ecbiz111.inmotionhosting.com</t>
-  </si>
-  <si>
     <t>Allowed Host</t>
   </si>
   <si>
     <t>Nickname</t>
   </si>
   <si>
-    <t>Winter's apartment</t>
-  </si>
-  <si>
-    <t>Newark, NJ Verizon.net</t>
-  </si>
-  <si>
     <t>Stevens</t>
   </si>
   <si>
@@ -114,22 +54,10 @@
     <t>Indiana University</t>
   </si>
   <si>
-    <t>NYC business?</t>
-  </si>
-  <si>
-    <t>Washington State (Asaf?)</t>
-  </si>
-  <si>
     <t>inMotion vps2933</t>
   </si>
   <si>
-    <t>inmotion ecbiz111</t>
-  </si>
-  <si>
-    <t>Maryland Comcast</t>
-  </si>
-  <si>
-    <t>New Orleans</t>
+    <t>Priscilla's</t>
   </si>
 </sst>
 </file>
@@ -219,8 +147,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -590,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -603,187 +532,58 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>